<commit_message>
# Add QR IMage to MQLThung Excell Print
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A069-IUNVW-1" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A075-FABIP-1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A069-IUNVW-1'!$A$1:$F$41]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A075-FABIP-1'!$A$1:$F$41]]></definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,16 +91,16 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">METAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1157</t>
+    <t xml:space="preserve">BOSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBAT5A-9-12</t>
   </si>
   <si>
     <t xml:space="preserve">150 (PCS)</t>
   </si>
   <si>
-    <t xml:space="preserve">TTP-A069-IUNVW-1</t>
+    <t xml:space="preserve">TTP-A075-FABIP-1</t>
   </si>
 </sst>
 </file>
@@ -136,13 +136,6 @@
     </font>
     <font>
       <b/>
-      <sz val="26"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="28"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -208,6 +201,13 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -375,122 +375,122 @@
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -508,6 +508,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -830,7 +873,7 @@
   <dimension ref="B1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,136 +888,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:15" ht="33" customHeight="1" x14ac:dyDescent="0.55">
-      <c r="B2" s="22" t="s">
+    <row r="2" spans="2:15" ht="70.2" customHeight="1" x14ac:dyDescent="0.55">
+      <c r="B2" s="41"/>
+      <c r="C2" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="31"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="32"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="15"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="29"/>
+      <c r="E7" s="24"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="25"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="29"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="24"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="25"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="29"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="24"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="25"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="18" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="24"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="17"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="29"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="24"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="17"/>
+      <c r="G11" s="14"/>
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="19"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="29"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="17"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="18" t="s">
+      <c r="C13" s="17"/>
+      <c r="D13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="17"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="19"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="5" t="s">
         <v>18</v>
       </c>
@@ -983,30 +1026,30 @@
       <c r="O14" s="8"/>
     </row>
     <row r="15" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="19"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="19"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="9"/>
       <c r="F15" s="7"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="10"/>
       <c r="E16" s="11"/>
       <c r="F16" s="7"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
       <c r="F17" s="12"/>
       <c r="G17" s="4"/>
     </row>
@@ -1035,13 +1078,23 @@
     <row r="34" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E4"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="E10:E12"/>
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="G10:G13"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:B9"/>
@@ -1049,19 +1102,11 @@
     <mergeCell ref="D7:D9"/>
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E4"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="G10:G13"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
   </mergeCells>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="11" scale="60" orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
+  <pageSetup paperSize="11" scale="90" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
# Remove TienDoGCRow not use NVID
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A075-FABIP-1" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A073-QHBAY-1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A075-FABIP-1'!$A$1:$F$41]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A073-QHBAY-1'!$A$1:$F$41]]></definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -91,16 +91,16 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">BOSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VBAT5A-9-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">150 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A075-FABIP-1</t>
+    <t xml:space="preserve">BODY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VX021S-2S3-02F-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">187 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A073-QHBAY-1</t>
   </si>
 </sst>
 </file>
@@ -218,7 +218,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -242,57 +242,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -301,7 +251,33 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -309,30 +285,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -347,7 +299,118 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -356,24 +419,130 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -385,9 +554,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -395,107 +561,150 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Style 1" xfId="2" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -872,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="B1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -887,178 +1096,178 @@
     <col min="7" max="7" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:15" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:15" ht="70.2" customHeight="1" x14ac:dyDescent="0.55">
-      <c r="B2" s="41"/>
-      <c r="C2" s="30" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="38"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="24"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="24"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="39"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="19"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="24"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="19"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="15" t="s">
+      <c r="C10" s="23"/>
+      <c r="D10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="14"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="24"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="24"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="14"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="15" t="s">
+      <c r="C13" s="45"/>
+      <c r="D13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="14"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="5" t="s">
+      <c r="B14" s="47"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="4"/>
-      <c r="O14" s="8"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="16"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="7"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
+    <row r="17" spans="2:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="12"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="2:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="2:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
# Modify Excel Template
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -2,17 +2,17 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A073-QHBAY-1" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A075-VDTKG-2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A073-QHBAY-1'!$A$1:$F$41]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A075-VDTKG-2'!$B$2:$E$17]]></definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
@@ -24,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">①</t>
   </si>
@@ -88,19 +87,28 @@
 Produced by IWK Company in Vietnam</t>
   </si>
   <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
     <t xml:space="preserve">BODY</t>
   </si>
   <si>
-    <t xml:space="preserve">VX021S-2S3-02F-B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">187 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A073-QHBAY-1</t>
+    <t xml:space="preserve">VX021S-2S3-02F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">130 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A058-VUCVQ-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBAT5A-9-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A075-VDTKG-2</t>
   </si>
 </sst>
 </file>
@@ -149,13 +157,6 @@
     </font>
     <font>
       <b/>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -197,17 +198,25 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="28"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="2">
@@ -542,169 +551,163 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Style 1" xfId="2" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -721,6 +724,49 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>156884</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104588</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>948767</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>717177</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="9230" t="10679" r="9232" b="9708"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="313766" y="201706"/>
+          <a:ext cx="791883" cy="612589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -736,13 +782,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPr id="2" name="Picture 2" descr="Picture"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1081,225 +1127,212 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="B1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="34.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.21875" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
+    <col min="1" max="1" width="2.26953125" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" customWidth="1"/>
+    <col min="5" max="5" width="37.1796875" customWidth="1"/>
+    <col min="6" max="6" width="7.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="7.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" ht="70.2" customHeight="1" x14ac:dyDescent="0.55">
-      <c r="B2" s="31"/>
-      <c r="C2" s="32" t="s">
+    <row r="1" spans="2:15" ht="7.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B2" s="11"/>
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
+    <row r="3" spans="2:15" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="36" t="s">
+      <c r="C3" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="37"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="35"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
+    <row r="4" spans="2:15" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="43"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="35" t="s">
+    <row r="5" spans="2:15" ht="18.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="E5" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-    </row>
-    <row r="6" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="35"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="35" t="s">
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+    </row>
+    <row r="6" spans="2:15" ht="18.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="43"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="39"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="30"/>
-    </row>
-    <row r="8" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="35"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="39"/>
+      <c r="G7" s="31"/>
+    </row>
+    <row r="8" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="43"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="32"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" spans="2:15" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="35"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="39"/>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="43"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="40" t="s">
+      <c r="G9" s="31"/>
+    </row>
+    <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="44" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="23"/>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="41"/>
+      <c r="E10" s="26"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="40"/>
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="44"/>
       <c r="C11" s="24"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="42"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="27"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="40"/>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="44"/>
       <c r="C12" s="25"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="43"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="44" t="s">
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="2:15" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="45"/>
-      <c r="D13" s="12" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="46"/>
+      <c r="E13" s="12"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="47"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="46" t="s">
-        <v>18</v>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="2:15" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="46"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="36" t="s">
+        <v>21</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="2:15" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="48"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="49"/>
+    <row r="15" spans="2:15" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="47"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="6"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:15" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="50" t="s">
+    <row r="16" spans="2:15" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="51"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="6"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="52" t="s">
+    <row r="17" spans="2:7" ht="59.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="9"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="19.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="2:7" ht="31.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="2:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:7" ht="18.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="2:7" ht="18.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="2:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="32.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="2:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="2:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="22" spans="2:7" ht="18.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:7" ht="18.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="2:7" ht="21.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:7" ht="21.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:7" ht="21.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="34" ht="39" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E4"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
     <mergeCell ref="G10:G13"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:C15"/>
@@ -1312,10 +1345,23 @@
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup paperSize="11" scale="90" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="256" scale="45" orientation="landscape" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
# Convert Excell number value to circled number
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A075-VDTKG-2" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A069-MRERV-7" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A075-VDTKG-2'!$B$2:$E$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A069-MRERV-7'!$B$2:$E$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">①</t>
   </si>
@@ -99,16 +99,19 @@
     <t xml:space="preserve">TTP-A058-VUCVQ-1</t>
   </si>
   <si>
-    <t xml:space="preserve">BOSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VBAT5A-9-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A075-VDTKG-2</t>
+    <t xml:space="preserve">METAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A069-MRERV-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⑦</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1149,7 @@
     <row r="2" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="11"/>
       <c r="C2" s="15" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>

</xml_diff>

<commit_message>
# Create function User-DongThung
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A069-MRERV-7" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A089-ETFHM-1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A069-MRERV-7'!$B$2:$E$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A089-ETFHM-1'!$B$2:$E$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t xml:space="preserve">①</t>
   </si>
@@ -99,19 +99,16 @@
     <t xml:space="preserve">TTP-A058-VUCVQ-1</t>
   </si>
   <si>
-    <t xml:space="preserve">METAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A069-MRERV-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">⑦</t>
+    <t xml:space="preserve">JOINT METAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1197-435-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A089-ETFHM-1</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1146,7 @@
     <row r="2" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B2" s="11"/>
       <c r="C2" s="15" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>

</xml_diff>

<commit_message>
# Change MQLThungTPExcelForm ( change write position )
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A089-ETFHM-1" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A074-YBPNQ-3" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A089-ETFHM-1'!$B$2:$E$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A074-YBPNQ-3'!$B$2:$E$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t xml:space="preserve">①</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Tên sản phẩm
 品名</t>
@@ -68,18 +65,10 @@
 重量</t>
   </si>
   <si>
-    <t xml:space="preserve">LOT　GC
-ロットNo.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nhân viên kiêm tra 
 検査員</t>
   </si>
   <si>
-    <t xml:space="preserve">LOT NL
-材料ロット</t>
-  </si>
-  <si>
     <t xml:space="preserve">PNo:  </t>
   </si>
   <si>
@@ -99,16 +88,26 @@
     <t xml:space="preserve">TTP-A058-VUCVQ-1</t>
   </si>
   <si>
-    <t xml:space="preserve">JOINT METAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H1197-435-00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A089-ETFHM-1</t>
+    <t xml:space="preserve">QR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#.......</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mã quản lý lot
+ロット管理No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BOSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VBAT5A-1-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">191 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A074-YBPNQ-3</t>
   </si>
 </sst>
 </file>
@@ -119,7 +118,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;KG&quot;"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +216,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="163"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -356,30 +361,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -539,6 +520,36 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -577,131 +588,131 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -724,71 +735,28 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>156884</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>104588</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>948767</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>717177</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Picture">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="9230" t="10679" r="9232" b="9708"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="313766" y="201706"/>
-          <a:ext cx="791883" cy="612589"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 2" descr="Picture"/>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1128,215 +1096,226 @@
   <dimension ref="B1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G10" sqref="G10:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.26953125" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" customWidth="1"/>
-    <col min="3" max="3" width="25.26953125" customWidth="1"/>
-    <col min="4" max="4" width="24.7265625" customWidth="1"/>
-    <col min="5" max="5" width="37.1796875" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" customWidth="1"/>
-    <col min="7" max="7" width="20.26953125" customWidth="1"/>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="7.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="11"/>
-      <c r="C2" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
+    <row r="1" spans="2:15" ht="7.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="49"/>
+      <c r="C2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="48"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="43" t="s">
+    <row r="3" spans="2:15" ht="32.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="42"/>
+      <c r="E3" s="44"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="2:15" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="43"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
+    <row r="4" spans="2:15" ht="32.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:15" ht="18.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="43" t="s">
+    <row r="5" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="48" t="s">
+      <c r="E5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="2:15" ht="18.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+    </row>
+    <row r="7" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-    </row>
-    <row r="6" spans="2:15" ht="18.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="43"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-    </row>
-    <row r="7" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="43" t="s">
+      <c r="C7" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="18" t="s">
+      <c r="E7" s="31"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="31"/>
-    </row>
-    <row r="8" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="43"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="31"/>
-    </row>
-    <row r="9" spans="2:15" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="43"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="31"/>
-    </row>
-    <row r="10" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="44" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="50"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="29"/>
-    </row>
-    <row r="11" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="44"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="44"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="29"/>
-    </row>
-    <row r="13" spans="2:15" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="12"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="29"/>
-    </row>
-    <row r="14" spans="2:15" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="46"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="36" t="s">
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="18"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="2:15" ht="21.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="47"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="13"/>
+    <row r="15" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="6"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="2:15" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="22"/>
+    <row r="16" spans="2:15" ht="32.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="42"/>
       <c r="D16" s="10"/>
-      <c r="E16" s="14"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="6"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="2:7" ht="59.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="35"/>
+    <row r="17" spans="2:7" ht="59.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
       <c r="F17" s="9"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="2:7" ht="19.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:7" ht="19.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="2:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="2:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="2:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="2:7" ht="18.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="2:7" ht="18.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="2:7" ht="21.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:7" ht="21.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="2:7" ht="21.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="32.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="39" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:7" ht="32.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:7" ht="32.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:7" ht="18.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:7" ht="18.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:7" ht="21.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="32.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="39" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="23">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
     <mergeCell ref="G10:G13"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:B9"/>
@@ -1345,19 +1324,6 @@
     <mergeCell ref="E7:E9"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:E4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
# Add Logo and Company Name
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A074-YBPNQ-3" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A107-RWRWP-3" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A074-YBPNQ-3'!$B$2:$E$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A107-RWRWP-3'!$B$2:$E$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t xml:space="preserve">Tên sản phẩm
 品名</t>
@@ -98,16 +98,13 @@
 ロット管理No</t>
   </si>
   <si>
-    <t xml:space="preserve">BOSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VBAT5A-1-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">191 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A074-YBPNQ-3</t>
+    <t xml:space="preserve">Khớp nối</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P5053-502-3F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A107-RWRWP-3</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1171,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>6</v>
@@ -1242,7 +1239,7 @@
       <c r="C14" s="46"/>
       <c r="D14" s="21"/>
       <c r="E14" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>

</xml_diff>

<commit_message>
# Handle ThungTTP odd-numbered
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A107-RWRWP-3" sheetId="1" r:id="rId1"/>
+    <sheet name="TTP-A032-NSVHT-4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A107-RWRWP-3'!$B$2:$E$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A032-NSVHT-4'!$B$2:$E$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Tên sản phẩm
 品名</t>
@@ -101,10 +101,13 @@
     <t xml:space="preserve">Khớp nối</t>
   </si>
   <si>
-    <t xml:space="preserve">P5053-502-3F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A107-RWRWP-3</t>
+    <t xml:space="preserve">P5053-502-4F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">89 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A032-NSVHT-4</t>
   </si>
 </sst>
 </file>
@@ -1171,7 +1174,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>6</v>
@@ -1239,7 +1242,7 @@
       <c r="C14" s="46"/>
       <c r="D14" s="21"/>
       <c r="E14" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="4"/>

</xml_diff>

<commit_message>
# Modify UI in DongThung Page
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A059-ENDFP-4" sheetId="3" r:id="rId1"/>
+    <sheet name="TTP-A110-UNCDO-1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A059-ENDFP-4'!$B$2:$G$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A110-UNCDO-1'!$B$2:$G$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -89,13 +89,13 @@
     <t xml:space="preserve">P5053-502-4F</t>
   </si>
   <si>
-    <t xml:space="preserve">32 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A059-ENDFP-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">④</t>
+    <t xml:space="preserve">130 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A110-UNCDO-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">①</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
# Ghep thung thanh pham ton kho
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A110-UNCDO-1" sheetId="3" r:id="rId1"/>
+    <sheet name="TTP-A059-TQHEF-1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A110-UNCDO-1'!$B$2:$G$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A059-TQHEF-1'!$B$2:$G$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">130 (PCS)</t>
   </si>
   <si>
-    <t xml:space="preserve">TTP-A110-UNCDO-1</t>
+    <t xml:space="preserve">TTP-A059-TQHEF-1</t>
   </si>
   <si>
     <t xml:space="preserve">①</t>

</xml_diff>

<commit_message>
# Modify Delete ThungTP Function - part2
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A059-TQHEF-1" sheetId="3" r:id="rId1"/>
+    <sheet name="TTP-A059-BRFQH-2" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A059-TQHEF-1'!$B$2:$G$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A059-BRFQH-2'!$B$2:$G$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -89,13 +89,13 @@
     <t xml:space="preserve">P5053-502-4F</t>
   </si>
   <si>
-    <t xml:space="preserve">130 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A059-TQHEF-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">①</t>
+    <t xml:space="preserve">120 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A059-BRFQH-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">②</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
# Fix miss searching if key change fast
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A059-BRFQH-2" sheetId="3" r:id="rId1"/>
+    <sheet name="TTP-A110-WILSQ-1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A059-BRFQH-2'!$B$2:$G$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A110-WILSQ-1'!$B$2:$G$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -89,13 +89,13 @@
     <t xml:space="preserve">P5053-502-4F</t>
   </si>
   <si>
-    <t xml:space="preserve">120 (PCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TTP-A059-BRFQH-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">②</t>
+    <t xml:space="preserve">130 (PCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A110-WILSQ-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">①</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
# Add Default Infor print QR function
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -7,10 +7,10 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="TTP-A110-WILSQ-1" sheetId="3" r:id="rId1"/>
+    <sheet name="TTP-A110-MLQQB-1" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A110-WILSQ-1'!$B$2:$G$17]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['TTP-A110-MLQQB-1'!$B$2:$G$17]]></definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t xml:space="preserve">Tên sản phẩm
 品名</t>
@@ -92,10 +92,16 @@
     <t xml:space="preserve">130 (PCS)</t>
   </si>
   <si>
-    <t xml:space="preserve">TTP-A110-WILSQ-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">①</t>
+    <t xml:space="preserve">30 KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/06/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTP-A110-MLQQB-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4</t>
   </si>
 </sst>
 </file>
@@ -484,6 +490,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,59 +568,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -950,7 +956,7 @@
   <dimension ref="B1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,133 +974,137 @@
   <sheetData>
     <row r="1" spans="2:17" ht="7.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="17"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:17" ht="87" customHeight="1" x14ac:dyDescent="0.55">
       <c r="B3" s="11"/>
       <c r="C3" s="1"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="19"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.55">
-      <c r="B4" s="42"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="35"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="23" t="s">
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="25"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:17" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="24" t="s">
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="27" t="s">
+      <c r="G7" s="42" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="30"/>
       <c r="I7" s="30"/>
     </row>
     <row r="8" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="33"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
     </row>
     <row r="9" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="32"/>
+      <c r="G9" s="43" t="s">
+        <v>17</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="30"/>
     </row>
     <row r="10" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="33"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="31"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="32"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="43"/>
       <c r="H10" s="3"/>
       <c r="I10" s="30"/>
     </row>
     <row r="11" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="33"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="31"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="32"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="43"/>
       <c r="H11" s="3"/>
       <c r="I11" s="30"/>
     </row>
     <row r="12" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="26" t="s">
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="14"/>
@@ -1102,61 +1112,61 @@
       <c r="I12" s="28"/>
     </row>
     <row r="13" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="33"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="26"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="14"/>
       <c r="H13" s="3"/>
       <c r="I13" s="28"/>
     </row>
     <row r="14" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="29"/>
-      <c r="F14" s="26"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="13"/>
       <c r="H14" s="5"/>
       <c r="I14" s="28"/>
     </row>
     <row r="15" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="33"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="29"/>
-      <c r="F15" s="26"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="4"/>
       <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="2:17" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="6"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="2:9" ht="34.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="26"/>
       <c r="H17" s="9"/>
       <c r="I17" s="4"/>
     </row>
@@ -1189,17 +1199,13 @@
     <row r="34" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D6"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="B9:D11"/>
-    <mergeCell ref="B12:D13"/>
-    <mergeCell ref="B14:D15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F2:G4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="I12:I14"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="H7:H8"/>
@@ -1208,13 +1214,17 @@
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="I9:I11"/>
-    <mergeCell ref="F2:G4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="B12:D13"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D6"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="B9:D11"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
# Add more field for PhieuHienPham
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t xml:space="preserve">Tên sản phẩm
 品名</t>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t xml:space="preserve">30 KG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TÔN TẤN KHANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PNo: 0703569660</t>
   </si>
   <si>
     <t xml:space="preserve">24/06/2025</t>
@@ -112,7 +118,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;KG&quot;"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,6 +225,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -232,7 +245,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -336,7 +349,7 @@
       <right style="medium">
         <color theme="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color theme="1"/>
       </top>
       <bottom style="thin">
@@ -345,13 +358,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color theme="1"/>
       </left>
       <right style="thin">
         <color theme="1"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color theme="1"/>
       </top>
       <bottom style="thin">
@@ -363,82 +376,86 @@
       <left style="thin">
         <color theme="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color theme="1"/>
       </right>
       <top style="thin">
         <color theme="1"/>
       </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
+      <left/>
+      <right style="medium">
         <color theme="1"/>
       </right>
       <top/>
       <bottom style="thin">
         <color theme="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="thin">
-        <color theme="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -449,7 +466,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -481,14 +498,62 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -502,52 +567,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -556,22 +588,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -956,7 +979,7 @@
   <dimension ref="B1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -974,199 +997,201 @@
   <sheetData>
     <row r="1" spans="2:17" ht="7.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="36"/>
-      <c r="F2" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="33"/>
+      <c r="F2" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="38"/>
     </row>
     <row r="3" spans="2:17" ht="87" customHeight="1" x14ac:dyDescent="0.55">
       <c r="B3" s="11"/>
       <c r="C3" s="1"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.55">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="44"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="39" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="41"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:17" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="40" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="31" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="43" t="s">
-        <v>17</v>
+      <c r="G9" s="24" t="s">
+        <v>19</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="30"/>
+      <c r="I9" s="22"/>
     </row>
     <row r="10" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="43"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="30"/>
+      <c r="I10" s="22"/>
     </row>
     <row r="11" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="43"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="24"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="30"/>
+      <c r="I11" s="22"/>
     </row>
     <row r="12" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="27" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="19" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="28"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="21"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="14"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="28"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="19"/>
       <c r="G14" s="13"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="28"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="4"/>
       <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="2:17" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="B16" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="6"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="2:9" ht="34.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="26"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="9"/>
       <c r="I17" s="4"/>
     </row>
@@ -1198,14 +1223,18 @@
     <row r="33" ht="32.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="39" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="F2:G4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+  <mergeCells count="25">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D6"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="B9:D11"/>
+    <mergeCell ref="B12:D13"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F15"/>
     <mergeCell ref="I12:I14"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="H7:H8"/>
@@ -1214,17 +1243,12 @@
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="I9:I11"/>
-    <mergeCell ref="B12:D13"/>
-    <mergeCell ref="B14:D15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D6"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="B9:D11"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:G6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E2:G4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
# Fix IDThung Address
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/MQLThungTPExcelForm.xlsx
@@ -95,10 +95,10 @@
     <t xml:space="preserve">30 KG</t>
   </si>
   <si>
-    <t xml:space="preserve">TÔN TẤN KHANG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PNo: 0703569660</t>
+    <t xml:space="preserve">KHANG TÔN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PNo: 2938109482</t>
   </si>
   <si>
     <t xml:space="preserve">24/06/2025</t>
@@ -507,6 +507,30 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -519,6 +543,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -567,34 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,7 +979,7 @@
   <dimension ref="B1:R34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="E2" sqref="E2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,173 +997,173 @@
   <sheetData>
     <row r="1" spans="2:17" ht="7.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37" t="s">
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="38"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="2:17" ht="87" customHeight="1" x14ac:dyDescent="0.55">
       <c r="B3" s="11"/>
       <c r="C3" s="1"/>
       <c r="D3" s="10"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="20"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:17" ht="3.6" customHeight="1" x14ac:dyDescent="0.55">
-      <c r="B4" s="34"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="44"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="2:17" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="16" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="2:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="25"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:17" ht="18.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="17" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
     </row>
     <row r="8" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="25"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
     </row>
     <row r="9" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="23" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="33" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="22"/>
+      <c r="I9" s="31"/>
     </row>
     <row r="10" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="25"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="24"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="22"/>
+      <c r="I10" s="31"/>
     </row>
     <row r="11" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="25"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="24"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="22"/>
+      <c r="I11" s="31"/>
     </row>
     <row r="12" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="31" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="27" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="20"/>
+      <c r="I12" s="29"/>
     </row>
     <row r="13" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="25"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="14"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="20"/>
+      <c r="I13" s="29"/>
     </row>
     <row r="14" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="21" t="s">
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="27"/>
       <c r="G14" s="13"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="20"/>
+      <c r="I14" s="29"/>
     </row>
     <row r="15" spans="2:17" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="25"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="19"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="27"/>
       <c r="G15" s="13" t="s">
         <v>20</v>
       </c>
@@ -1172,26 +1172,26 @@
       <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="2:17" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
       <c r="F16" s="12"/>
       <c r="G16" s="15"/>
       <c r="H16" s="6"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="2:9" ht="34.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="9"/>
       <c r="I17" s="4"/>
     </row>
@@ -1243,12 +1243,12 @@
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="G9:G11"/>
     <mergeCell ref="I9:I11"/>
+    <mergeCell ref="E2:G4"/>
     <mergeCell ref="E5:E6"/>
     <mergeCell ref="F5:G6"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E2:G4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>